<commit_message>
test vehicle configuration completed
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C72BCB-C543-4D97-9F36-6BE5E64A3C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD2845-4D82-490E-BD19-84A63D83D222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8A4A79A-A8FC-40C7-8B12-FB303BD05A6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8A4A79A-A8FC-40C7-8B12-FB303BD05A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="doSignIn" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="doSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>email</t>
   </si>
@@ -65,6 +65,27 @@
   </si>
   <si>
     <t>Qwerty2023/*-</t>
+  </si>
+  <si>
+    <t>BMW M4</t>
+  </si>
+  <si>
+    <t>BMW M8</t>
+  </si>
+  <si>
+    <t>BMW X2</t>
+  </si>
+  <si>
+    <t>BMW X5</t>
+  </si>
+  <si>
+    <t>BMW i4</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -435,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160DC7EC-0A9F-44B8-9EB1-27A0B115CF7E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -502,12 +523,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA639A3-CE81-400B-BB24-E1BE3F541431}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test search and test
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD2845-4D82-490E-BD19-84A63D83D222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8240519E-2036-4418-B444-16040E8AE867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8A4A79A-A8FC-40C7-8B12-FB303BD05A6C}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA639A3-CE81-400B-BB24-E1BE3F541431}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>